<commit_message>
Added test cases and icon in the panel
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C1D456C-9704-437C-AE4C-30584E0124CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E1633-03B9-4F3B-A0E7-ABC77989C14A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -433,6 +433,25 @@
   </si>
   <si>
     <t>P1 is highest priority and P5 is lowest.</t>
+  </si>
+  <si>
+    <t>TC-22</t>
+  </si>
+  <si>
+    <t>Functionality 
+Testing</t>
+  </si>
+  <si>
+    <t>Verify that Clear Enteries button working fine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> application is opened and has been used atleast once</t>
+  </si>
+  <si>
+    <t>1. Press Clear Enteries Button</t>
+  </si>
+  <si>
+    <t>All input Fields as well as output fields should get clear</t>
   </si>
 </sst>
 </file>
@@ -556,9 +575,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -590,6 +606,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -944,740 +963,772 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="I3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="9"/>
+      <c r="I4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="I6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="I8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="I9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="I10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="I11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="I12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="I13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="7" t="s">
+      <c r="I14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="7" t="s">
+      <c r="I15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="7" t="s">
+      <c r="I16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="7" t="s">
+      <c r="I17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="7" t="s">
+      <c r="I18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="7" t="s">
+      <c r="I19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="7" t="s">
+      <c r="I20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="7" t="s">
+      <c r="I21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="7" t="s">
+      <c r="I22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="I23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="7" t="s">
+      <c r="I23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1702,16 +1753,16 @@
       <c r="D29" s="16"/>
     </row>
     <row r="1048576" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1048576" s="3"/>
-      <c r="B1048576" s="3"/>
-      <c r="C1048576" s="3"/>
-      <c r="D1048576" s="4"/>
-      <c r="E1048576" s="4"/>
-      <c r="F1048576" s="5"/>
-      <c r="G1048576" s="4"/>
-      <c r="H1048576" s="4"/>
-      <c r="I1048576" s="6"/>
-      <c r="J1048576" s="3"/>
+      <c r="A1048576" s="2"/>
+      <c r="B1048576" s="2"/>
+      <c r="C1048576" s="2"/>
+      <c r="D1048576" s="3"/>
+      <c r="E1048576" s="3"/>
+      <c r="F1048576" s="4"/>
+      <c r="G1048576" s="3"/>
+      <c r="H1048576" s="3"/>
+      <c r="I1048576" s="5"/>
+      <c r="J1048576" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>